<commit_message>
added coverage for edge cases
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/Data.xlsx
+++ b/src/test/resources/ExcelData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/likitha.lokesh/java-selenium-cucumber/src/test/resources/ExcelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF52C95F-E507-1B4A-AF6A-04B9715ABDA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEC9A79-9024-E74C-A68A-B0ECBDAAE9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{2650AA53-9C0B-C546-9058-C75D041CBE5A}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
-    <t>likithal39@gmail.com</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -48,6 +45,9 @@
   </si>
   <si>
     <t>Sun$Daisy132</t>
+  </si>
+  <si>
+    <t>likitha.lokesh@slalom.com</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,10 +466,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -482,10 +482,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
@@ -498,10 +498,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
@@ -514,10 +514,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>

</xml_diff>